<commit_message>
autodock & vina completed
</commit_message>
<xml_diff>
--- a/autodock/res.xlsx
+++ b/autodock/res.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="A-amylase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="34">
   <si>
     <t>Anestezin</t>
   </si>
@@ -571,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J15"/>
     </sheetView>
   </sheetViews>
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,13 +1448,15 @@
     <col min="8" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
+    <row r="2" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -2711,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,7 +2990,7 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="2">
@@ -3134,6 +3136,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3570,7 +3573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>